<commit_message>
Took Task 3 and Task 4
</commit_message>
<xml_diff>
--- a/TasksList.xlsx
+++ b/TasksList.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gemini Repo\Gemini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="86">
   <si>
     <t>Notes</t>
   </si>
@@ -448,6 +453,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -495,7 +503,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,7 +538,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,8 +940,8 @@
       <c r="B18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>77</v>
+      <c r="C18" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>83</v>
@@ -964,8 +972,8 @@
       <c r="B21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>77</v>
+      <c r="C21" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>83</v>
@@ -973,7 +981,9 @@
       <c r="E21" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G21" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Updated the task list for DE-39-MF task
</commit_message>
<xml_diff>
--- a/TasksList.xlsx
+++ b/TasksList.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gemini Repo\Gemini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -503,7 +498,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,7 +533,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,8 +1659,8 @@
       <c r="B66" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C66" s="11" t="s">
-        <v>76</v>
+      <c r="C66" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>77</v>

</xml_diff>